<commit_message>
querrys toegevoegd & timeTable aangepast
</commit_message>
<xml_diff>
--- a/Time Table.xlsx
+++ b/Time Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RubenClaes/Documents/Ucll/1_S2/Databanken &amp; Dataquerying/GroepsWerkGit/GroepsWerk_Nature_SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C2F3A8-4465-114C-98F5-122E2DD3475E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC95D4E-69F1-A243-BBBD-BB83EE6DD088}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="440" windowWidth="27640" windowHeight="16140" xr2:uid="{0111D7EB-AF11-5B43-947A-691B85D3BAD9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
   <si>
     <t>Week2</t>
   </si>
@@ -320,7 +320,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -338,7 +338,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -376,7 +376,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -482,7 +482,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBAAB67-AB22-2743-9694-6543EECBEB62}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="L4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1163,10 +1163,10 @@
         <v>33</v>
       </c>
       <c r="H18" s="7">
-        <v>2</v>
-      </c>
-      <c r="I18" s="8">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="9"/>
@@ -1175,7 +1175,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="8"/>
       <c r="P18" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>